<commit_message>
Sync and increase box collider size
</commit_message>
<xml_diff>
--- a/Reports/Execution Plan/execution_timeline.xlsx
+++ b/Reports/Execution Plan/execution_timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick1\Documents\TAMU\2020_Fall\ECEN 403-904\Reports\Execution Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920AF2AB-4046-4AA9-9807-2E52BE9802E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F792E589-1ED6-4CB3-9A72-4C1ACF052CB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C0A2AB5C-EB32-468C-B509-75EBA033E64A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C0A2AB5C-EB32-468C-B509-75EBA033E64A}"/>
   </bookViews>
   <sheets>
     <sheet name="Execution Timeline" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t>Status update 3</t>
   </si>
@@ -248,10 +248,6 @@
   </si>
   <si>
     <t>COMPLETE</t>
-  </si>
-  <si>
-    <t>ONGOING, rudimentary test complete, but still
-need to verify accuracy</t>
   </si>
   <si>
     <t>Status Update 5</t>
@@ -735,7 +731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D856D392-E2BA-4602-A97D-75A3FF643628}">
   <dimension ref="B7:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
@@ -1020,7 +1016,7 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1099,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE4086C-BF2C-45C0-B49D-FCF44CD9C55B}">
   <dimension ref="B3:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,7 +1149,7 @@
         <v>26</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>25</v>
@@ -1174,7 +1170,7 @@
         <v>67</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>30</v>
@@ -1256,7 +1252,7 @@
         <v>66</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>39</v>
@@ -1348,7 +1344,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="22"/>
       <c r="C14" s="1" t="s">
         <v>60</v>
@@ -1360,7 +1356,7 @@
         <v>62</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G14" s="2">
         <v>44264</v>

</xml_diff>